<commit_message>
Added ID for cycling cell
</commit_message>
<xml_diff>
--- a/cell_ontology.xlsx
+++ b/cell_ontology.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="169">
   <si>
     <t xml:space="preserve">cell_ontology</t>
   </si>
@@ -510,6 +510,15 @@
   </si>
   <si>
     <t xml:space="preserve">T CD4 eff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cycling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cycl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cycling</t>
   </si>
 </sst>
 </file>
@@ -2261,6 +2270,26 @@
         <v>17</v>
       </c>
     </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>166</v>
+      </c>
+      <c r="B72" t="s">
+        <v>167</v>
+      </c>
+      <c r="C72" t="s">
+        <v>168</v>
+      </c>
+      <c r="D72" t="s">
+        <v>168</v>
+      </c>
+      <c r="E72" t="s">
+        <v>168</v>
+      </c>
+      <c r="F72" t="s">
+        <v>168</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>